<commit_message>
Added all the Activities and all Goal and the Student in Members
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/LearningTree.xlsx
+++ b/src/test/resources/ExcelFiles/LearningTree.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FPK_Automation_Scripts\LT_Automation\src\test\resources\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69550CCE-C85E-478C-B8B8-98B2E3396E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09076D79-232C-423B-998D-7DE47C1EFEAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STAGE" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="43">
   <si>
     <t>FirstName</t>
   </si>
@@ -125,64 +125,31 @@
     <t>CourseDesignerName</t>
   </si>
   <si>
-    <t>CourseDesigner36539</t>
-  </si>
-  <si>
-    <t>LearningCourse1560</t>
-  </si>
-  <si>
     <t>LearningCourseName</t>
   </si>
   <si>
-    <t>CourseDesigner55151</t>
-  </si>
-  <si>
-    <t>CourseDesigner16316</t>
-  </si>
-  <si>
-    <t>CourseDesigner49443</t>
-  </si>
-  <si>
-    <t>LearningCourse91958</t>
-  </si>
-  <si>
-    <t>CourseDesigner42850</t>
-  </si>
-  <si>
-    <t>LearningCourse92699</t>
-  </si>
-  <si>
-    <t>CourseDesigner90178</t>
-  </si>
-  <si>
-    <t>CourseDesigner18292</t>
-  </si>
-  <si>
-    <t>LearningCourse76663</t>
-  </si>
-  <si>
-    <t>LearningCourse72272</t>
-  </si>
-  <si>
-    <t>LearningCourse27539</t>
-  </si>
-  <si>
-    <t>CourseDesigner89132</t>
-  </si>
-  <si>
-    <t>LearningCourse51606</t>
-  </si>
-  <si>
-    <t>CourseDesigner48347</t>
-  </si>
-  <si>
-    <t>LearningCourse53991</t>
-  </si>
-  <si>
-    <t>CourseDesigner49515</t>
-  </si>
-  <si>
-    <t>LearningCourse76350</t>
+    <t>CourseDesigner91070</t>
+  </si>
+  <si>
+    <t>LearningCourse43256</t>
+  </si>
+  <si>
+    <t>LearningCourse75620</t>
+  </si>
+  <si>
+    <t>LearningCourse6712</t>
+  </si>
+  <si>
+    <t>LearningCourse31250</t>
+  </si>
+  <si>
+    <t>LearningCourse30346</t>
+  </si>
+  <si>
+    <t>LearningCourse2517</t>
+  </si>
+  <si>
+    <t>LearningCourse66017</t>
   </si>
 </sst>
 </file>
@@ -252,7 +219,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -324,6 +291,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <bottom style="thin"/>
     </border>
     <border>
@@ -335,7 +313,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -393,55 +371,25 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
     </xf>
   </cellXfs>
@@ -751,8 +699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -807,7 +755,7 @@
         <v>33</v>
       </c>
       <c r="L1" s="19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="M1" s="9"/>
     </row>
@@ -842,11 +790,11 @@
       <c r="J2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="K2" t="s" s="36">
-        <v>52</v>
-      </c>
-      <c r="L2" t="s" s="37">
-        <v>53</v>
+      <c r="K2" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" t="s" s="27">
+        <v>42</v>
       </c>
       <c r="M2" s="9"/>
       <c r="N2" s="9"/>
@@ -943,7 +891,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -996,7 +944,7 @@
         <v>33</v>
       </c>
       <c r="L1" s="19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="M1" s="9"/>
     </row>

</xml_diff>

<commit_message>
Latest code for provide score for all Activities
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/LearningTree.xlsx
+++ b/src/test/resources/ExcelFiles/LearningTree.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="114">
   <si>
     <t>FirstName</t>
   </si>
@@ -207,6 +207,162 @@
   </si>
   <si>
     <t>LearningCourse68375</t>
+  </si>
+  <si>
+    <t>CourseDesigner28585</t>
+  </si>
+  <si>
+    <t>LearningCourse78086</t>
+  </si>
+  <si>
+    <t>LearningCourse94485</t>
+  </si>
+  <si>
+    <t>LearningCourse20218</t>
+  </si>
+  <si>
+    <t>LearningCourse91080</t>
+  </si>
+  <si>
+    <t>LearningCourse37730</t>
+  </si>
+  <si>
+    <t>LearningCourse54521</t>
+  </si>
+  <si>
+    <t>LearningCourse31088</t>
+  </si>
+  <si>
+    <t>CourseDesigner74085</t>
+  </si>
+  <si>
+    <t>CourseDesigner53928</t>
+  </si>
+  <si>
+    <t>LearningCourse15901</t>
+  </si>
+  <si>
+    <t>LearningCourse90690</t>
+  </si>
+  <si>
+    <t>LearningCourse94765</t>
+  </si>
+  <si>
+    <t>LearningCourse93887</t>
+  </si>
+  <si>
+    <t>LearningCourse83527</t>
+  </si>
+  <si>
+    <t>LearningCourse38715</t>
+  </si>
+  <si>
+    <t>LearningCourse6601</t>
+  </si>
+  <si>
+    <t>LearningCourse6796</t>
+  </si>
+  <si>
+    <t>LearningCourse25056</t>
+  </si>
+  <si>
+    <t>LearningCourse12273</t>
+  </si>
+  <si>
+    <t>CourseDesigner24460</t>
+  </si>
+  <si>
+    <t>LearningCourse52945</t>
+  </si>
+  <si>
+    <t>LearningCourse89094</t>
+  </si>
+  <si>
+    <t>CourseDesigner58541</t>
+  </si>
+  <si>
+    <t>LearningCourse99575</t>
+  </si>
+  <si>
+    <t>LearningCourse55246</t>
+  </si>
+  <si>
+    <t>LearningCourse45946</t>
+  </si>
+  <si>
+    <t>LearningCourse77515</t>
+  </si>
+  <si>
+    <t>LearningCourse89776</t>
+  </si>
+  <si>
+    <t>LearningCourse69948</t>
+  </si>
+  <si>
+    <t>LearningCourse24970</t>
+  </si>
+  <si>
+    <t>LearningCourse45297</t>
+  </si>
+  <si>
+    <t>LearningCourse56646</t>
+  </si>
+  <si>
+    <t>LearningCourse15099</t>
+  </si>
+  <si>
+    <t>LearningCourse34875</t>
+  </si>
+  <si>
+    <t>LearningCourse23083</t>
+  </si>
+  <si>
+    <t>LearningCourse41257</t>
+  </si>
+  <si>
+    <t>LearningCourse72502</t>
+  </si>
+  <si>
+    <t>LearningCourse60127</t>
+  </si>
+  <si>
+    <t>LearningCourse55148</t>
+  </si>
+  <si>
+    <t>LearningCourse94671</t>
+  </si>
+  <si>
+    <t>LearningCourse43711</t>
+  </si>
+  <si>
+    <t>LearningCourse23534</t>
+  </si>
+  <si>
+    <t>CourseDesigner66366</t>
+  </si>
+  <si>
+    <t>LearningCourse17407</t>
+  </si>
+  <si>
+    <t>CourseDesigner92640</t>
+  </si>
+  <si>
+    <t>LearningCourse96364</t>
+  </si>
+  <si>
+    <t>CourseDesigner16229</t>
+  </si>
+  <si>
+    <t>LearningCourse44276</t>
+  </si>
+  <si>
+    <t>LearningCourse68983</t>
+  </si>
+  <si>
+    <t>CourseDesigner70039</t>
+  </si>
+  <si>
+    <t>LearningCourse45781</t>
   </si>
 </sst>
 </file>
@@ -370,7 +526,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -430,6 +586,162 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
@@ -904,11 +1216,11 @@
       <c r="J2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="K2" t="s" s="28">
-        <v>43</v>
-      </c>
-      <c r="L2" t="s" s="46">
-        <v>61</v>
+      <c r="K2" t="s" s="97">
+        <v>112</v>
+      </c>
+      <c r="L2" t="s" s="98">
+        <v>113</v>
       </c>
       <c r="M2" s="9"/>
       <c r="N2" s="9"/>

</xml_diff>

<commit_message>
Changes did in Student side Activities submission
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/LearningTree.xlsx
+++ b/src/test/resources/ExcelFiles/LearningTree.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="154">
   <si>
     <t>FirstName</t>
   </si>
@@ -471,6 +471,18 @@
   </si>
   <si>
     <t>CourseDesigner61777</t>
+  </si>
+  <si>
+    <t>CourseDesigner99126</t>
+  </si>
+  <si>
+    <t>LearningCourse3395</t>
+  </si>
+  <si>
+    <t>CourseDesigner40081</t>
+  </si>
+  <si>
+    <t>LearningCourse39214</t>
   </si>
 </sst>
 </file>
@@ -634,7 +646,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -694,6 +706,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
@@ -1432,11 +1456,11 @@
       <c r="J2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="K2" t="s" s="134">
-        <v>149</v>
-      </c>
-      <c r="L2" t="s" s="131">
-        <v>146</v>
+      <c r="K2" t="s" s="137">
+        <v>152</v>
+      </c>
+      <c r="L2" t="s" s="138">
+        <v>153</v>
       </c>
       <c r="M2" s="9"/>
       <c r="N2" s="9"/>

</xml_diff>

<commit_message>
Latest Changes while provide the score for the Activities
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/LearningTree.xlsx
+++ b/src/test/resources/ExcelFiles/LearningTree.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="194">
   <si>
     <t>FirstName</t>
   </si>
@@ -600,6 +600,9 @@
   </si>
   <si>
     <t>LearningCourse80642</t>
+  </si>
+  <si>
+    <t>LearningCourse24490</t>
   </si>
 </sst>
 </file>
@@ -763,7 +766,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="178">
+  <cellXfs count="179">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -823,6 +826,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
@@ -1693,8 +1699,8 @@
       <c r="K2" t="s" s="175">
         <v>190</v>
       </c>
-      <c r="L2" t="s" s="177">
-        <v>192</v>
+      <c r="L2" t="s" s="178">
+        <v>193</v>
       </c>
       <c r="M2" s="9"/>
       <c r="N2" s="9"/>

</xml_diff>

<commit_message>
Latest Changes and also added the Report Card Functionality
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/LearningTree.xlsx
+++ b/src/test/resources/ExcelFiles/LearningTree.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="94">
   <si>
     <t>FirstName</t>
   </si>
@@ -210,6 +210,99 @@
   </si>
   <si>
     <t>LearningCourse62806</t>
+  </si>
+  <si>
+    <t>LearningCourse85388</t>
+  </si>
+  <si>
+    <t>CourseDesigner33199</t>
+  </si>
+  <si>
+    <t>CourseDesigner90565</t>
+  </si>
+  <si>
+    <t>LearningCourse16331</t>
+  </si>
+  <si>
+    <t>LearningCourse7092</t>
+  </si>
+  <si>
+    <t>LearningCourse83436</t>
+  </si>
+  <si>
+    <t>LearningCourse76170</t>
+  </si>
+  <si>
+    <t>CourseDesigner37205</t>
+  </si>
+  <si>
+    <t>LearningCourse4945</t>
+  </si>
+  <si>
+    <t>CourseDesigner23692</t>
+  </si>
+  <si>
+    <t>LearningCourse67576</t>
+  </si>
+  <si>
+    <t>LearningCourse18179</t>
+  </si>
+  <si>
+    <t>LearningCourse33665</t>
+  </si>
+  <si>
+    <t>CourseDesigner49754</t>
+  </si>
+  <si>
+    <t>LearningCourse85870</t>
+  </si>
+  <si>
+    <t>LearningCourse1814</t>
+  </si>
+  <si>
+    <t>LearningCourse52809</t>
+  </si>
+  <si>
+    <t>LearningCourse94095</t>
+  </si>
+  <si>
+    <t>LearningCourse94880</t>
+  </si>
+  <si>
+    <t>LearningCourse61439</t>
+  </si>
+  <si>
+    <t>LearningCourse62876</t>
+  </si>
+  <si>
+    <t>CourseDesigner57510</t>
+  </si>
+  <si>
+    <t>CourseDesigner47766</t>
+  </si>
+  <si>
+    <t>LearningCourse14429</t>
+  </si>
+  <si>
+    <t>CourseDesigner99542</t>
+  </si>
+  <si>
+    <t>CourseDesigner32161</t>
+  </si>
+  <si>
+    <t>LearningCourse65138</t>
+  </si>
+  <si>
+    <t>CourseDesigner67344</t>
+  </si>
+  <si>
+    <t>CourseDesigner49287</t>
+  </si>
+  <si>
+    <t>CourseDesigner86408</t>
+  </si>
+  <si>
+    <t>LearningCourse26984</t>
   </si>
 </sst>
 </file>
@@ -373,7 +466,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -433,6 +526,99 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
@@ -910,11 +1096,11 @@
       <c r="J2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="L2" s="21" t="s">
-        <v>35</v>
+      <c r="K2" t="s" s="77">
+        <v>92</v>
+      </c>
+      <c r="L2" t="s" s="78">
+        <v>93</v>
       </c>
       <c r="M2" s="9"/>
       <c r="N2" s="9"/>
@@ -1100,11 +1286,11 @@
       <c r="J2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K2" t="s" s="46">
-        <v>61</v>
-      </c>
-      <c r="L2" t="s" s="47">
-        <v>62</v>
+      <c r="K2" t="s" s="57">
+        <v>72</v>
+      </c>
+      <c r="L2" t="s" s="59">
+        <v>74</v>
       </c>
       <c r="M2" s="3"/>
     </row>

</xml_diff>